<commit_message>
added new step defs
</commit_message>
<xml_diff>
--- a/src/test/resources/com/prestashop/test-data/Products.xlsx
+++ b/src/test/resources/com/prestashop/test-data/Products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekschool/JavaPrgs/acceptance-tests/src/test/resources/com/prestashop/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF1A6AD-3BCB-2A4C-8231-02867251247A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B89288-83DF-8F49-AC1F-D554838A94FB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="20980" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Execute</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Blue</t>
   </si>
   <si>
-    <t>option</t>
-  </si>
-  <si>
     <t>Price: Lowest first</t>
   </si>
   <si>
@@ -142,10 +139,13 @@
     <t xml:space="preserve"> Printed Summer Dress             </t>
   </si>
   <si>
-    <t xml:space="preserve">price        </t>
-  </si>
-  <si>
-    <t>name</t>
+    <t xml:space="preserve">Price        </t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Option</t>
   </si>
 </sst>
 </file>
@@ -602,21 +602,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333419CA-489B-534C-9571-ABC48E4CE77F}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="256" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>38</v>
@@ -624,81 +624,108 @@
       <c r="C1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1">
+        <v>50.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D4" s="1">
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1">
-        <v>50.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D5" s="1">
+        <v>28.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1">
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1">
-        <v>28.98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="1">
-        <v>16.399999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>26</v>
       </c>
     </row>

</xml_diff>